<commit_message>
example of species replace/update file
</commit_message>
<xml_diff>
--- a/www/SpeciesReplace.xlsx
+++ b/www/SpeciesReplace.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tsgil\OneDrive\Documents\VGS\App-VGS-Batch-Importer\www\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EAE47B50-3E3E-444F-B28E-8CBFE4A9AF58}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50ABCFFF-385C-41F4-A1F9-7DCC4BEE49E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{E2EB6185-1D46-4667-8306-68408B08410E}"/>
+    <workbookView xWindow="19090" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{E2EB6185-1D46-4667-8306-68408B08410E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="29">
   <si>
     <t>OldCode</t>
   </si>
@@ -84,6 +84,45 @@
   </si>
   <si>
     <t>MAGL2</t>
+  </si>
+  <si>
+    <t>AGROP</t>
+  </si>
+  <si>
+    <t>AGRT</t>
+  </si>
+  <si>
+    <t>ANSE</t>
+  </si>
+  <si>
+    <t>ARA</t>
+  </si>
+  <si>
+    <t>HEHO</t>
+  </si>
+  <si>
+    <t>HOBR</t>
+  </si>
+  <si>
+    <t>AGTR</t>
+  </si>
+  <si>
+    <t>ANSE4</t>
+  </si>
+  <si>
+    <t>HEHO5</t>
+  </si>
+  <si>
+    <t>ARABI2</t>
+  </si>
+  <si>
+    <t>HOBR2</t>
+  </si>
+  <si>
+    <t>LYDR</t>
+  </si>
+  <si>
+    <t>LYDR2</t>
   </si>
 </sst>
 </file>
@@ -464,9 +503,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{43A2D61C-BF9C-430C-81F0-3E823A00CF18}">
-  <dimension ref="A1:B8"/>
+  <dimension ref="A1:B15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -483,57 +524,113 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>2</v>
+        <v>16</v>
       </c>
       <c r="B2" t="s">
-        <v>11</v>
+        <v>22</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>3</v>
+        <v>17</v>
       </c>
       <c r="B3" t="s">
-        <v>13</v>
+        <v>22</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>5</v>
+        <v>18</v>
       </c>
       <c r="B5" t="s">
-        <v>6</v>
+        <v>23</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>7</v>
+        <v>19</v>
       </c>
       <c r="B6" t="s">
-        <v>14</v>
+        <v>25</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="B7" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
+        <v>4</v>
+      </c>
+      <c r="B8" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>5</v>
+      </c>
+      <c r="B9" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>7</v>
+      </c>
+      <c r="B10" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>20</v>
+      </c>
+      <c r="B11" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>21</v>
+      </c>
+      <c r="B12" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>8</v>
+      </c>
+      <c r="B13" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>27</v>
+      </c>
+      <c r="B14" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
         <v>10</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B15" t="s">
         <v>15</v>
       </c>
     </row>

</xml_diff>

<commit_message>
sp lists only for local use - too much files
</commit_message>
<xml_diff>
--- a/www/SpeciesReplace.xlsx
+++ b/www/SpeciesReplace.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tsgil\OneDrive\Documents\VGS\App-VGS-Batch-Importer\www\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0B5CC35-F5BB-4723-B821-BC0040F5DB5D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DEE31813-9D27-4B75-8C74-1B80A862B431}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2990" yWindow="2650" windowWidth="14680" windowHeight="9740" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="19090" yWindow="-4490" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet 1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="3">
   <si>
     <t>OldCodes</t>
   </si>
@@ -28,16 +28,7 @@
     <t>NewCode</t>
   </si>
   <si>
-    <t>BRCA</t>
-  </si>
-  <si>
-    <t>HAFL</t>
-  </si>
-  <si>
-    <t>HAFL2</t>
-  </si>
-  <si>
-    <t>BRCA2</t>
+    <t/>
   </si>
 </sst>
 </file>
@@ -371,11 +362,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
@@ -388,19 +377,18 @@
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
+      <c r="B2" t="s">
         <v>2</v>
-      </c>
-      <c r="B2" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
-        <v>3</v>
-      </c>
       <c r="B3" t="s">
-        <v>4</v>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B4" t="s">
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fixes for LI insert and species replace update
</commit_message>
<xml_diff>
--- a/www/SpeciesReplace.xlsx
+++ b/www/SpeciesReplace.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tsgil\OneDrive\Documents\VGS\App-VGS-Batch-Importer\www\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tsgil\OneDrive\Documents\VGS - R\App-VGS-Batch-Importer\www\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DEE31813-9D27-4B75-8C74-1B80A862B431}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2D9ED30-EEC0-46AE-9652-C681A341515B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19090" yWindow="-4490" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-13700" yWindow="0" windowWidth="10620" windowHeight="8450" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet 1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="108">
   <si>
     <t>OldCodes</t>
   </si>
@@ -28,17 +28,345 @@
     <t>NewCode</t>
   </si>
   <si>
-    <t/>
+    <t>ACDA</t>
+  </si>
+  <si>
+    <t>ACMI</t>
+  </si>
+  <si>
+    <t>AGCA</t>
+  </si>
+  <si>
+    <t>ALPR</t>
+  </si>
+  <si>
+    <t>ARTR3</t>
+  </si>
+  <si>
+    <t>BECA2</t>
+  </si>
+  <si>
+    <t>CACH</t>
+  </si>
+  <si>
+    <t>CADE</t>
+  </si>
+  <si>
+    <t>CAIN13</t>
+  </si>
+  <si>
+    <t>CAPA</t>
+  </si>
+  <si>
+    <t>CAPE6</t>
+  </si>
+  <si>
+    <t>CASC</t>
+  </si>
+  <si>
+    <t>CASU</t>
+  </si>
+  <si>
+    <t>CATE24</t>
+  </si>
+  <si>
+    <t>CHNA2</t>
+  </si>
+  <si>
+    <t>DECA3</t>
+  </si>
+  <si>
+    <t>ELBR</t>
+  </si>
+  <si>
+    <t>ELEL</t>
+  </si>
+  <si>
+    <t>EPST</t>
+  </si>
+  <si>
+    <t>EROC</t>
+  </si>
+  <si>
+    <t>GAAP</t>
+  </si>
+  <si>
+    <t>GAPA</t>
+  </si>
+  <si>
+    <t>HYAN</t>
+  </si>
+  <si>
+    <t>JUCR</t>
+  </si>
+  <si>
+    <t>LANE</t>
+  </si>
+  <si>
+    <t>LINA</t>
+  </si>
+  <si>
+    <t>LOPE10</t>
+  </si>
+  <si>
+    <t>LOPU</t>
+  </si>
+  <si>
+    <t>MUFI</t>
+  </si>
+  <si>
+    <t>PHHE16</t>
+  </si>
+  <si>
+    <t>RAOC2</t>
+  </si>
+  <si>
+    <t>RAOR</t>
+  </si>
+  <si>
+    <t>ROAC2</t>
+  </si>
+  <si>
+    <t>ROSA</t>
+  </si>
+  <si>
+    <t>ROSE</t>
+  </si>
+  <si>
+    <t>RUCA</t>
+  </si>
+  <si>
+    <t>SCMI</t>
+  </si>
+  <si>
+    <t>SIAN3</t>
+  </si>
+  <si>
+    <t>SIEN</t>
+  </si>
+  <si>
+    <t>SOCA</t>
+  </si>
+  <si>
+    <t>TREP</t>
+  </si>
+  <si>
+    <t>TRER</t>
+  </si>
+  <si>
+    <t>TRRE</t>
+  </si>
+  <si>
+    <t>PODA</t>
+  </si>
+  <si>
+    <t>ACMI2</t>
+  </si>
+  <si>
+    <t>ALPR3</t>
+  </si>
+  <si>
+    <t>ARTR2</t>
+  </si>
+  <si>
+    <t>VECA2</t>
+  </si>
+  <si>
+    <t>CAEL</t>
+  </si>
+  <si>
+    <t>CADE27</t>
+  </si>
+  <si>
+    <t>CAIN</t>
+  </si>
+  <si>
+    <t>CAPA14</t>
+  </si>
+  <si>
+    <t>CAPE5</t>
+  </si>
+  <si>
+    <t>CASC7</t>
+  </si>
+  <si>
+    <t>CASU6</t>
+  </si>
+  <si>
+    <t>CATE26</t>
+  </si>
+  <si>
+    <t>ERNAN5</t>
+  </si>
+  <si>
+    <t>ERLA</t>
+  </si>
+  <si>
+    <t>ELIN7</t>
+  </si>
+  <si>
+    <t>ELEL5</t>
+  </si>
+  <si>
+    <t>EPILO</t>
+  </si>
+  <si>
+    <t>ERIGE2</t>
+  </si>
+  <si>
+    <t>GAAP2</t>
+  </si>
+  <si>
+    <t>GAPA5</t>
+  </si>
+  <si>
+    <t>HYAN2</t>
+  </si>
+  <si>
+    <t>JUOR</t>
+  </si>
+  <si>
+    <t>LANE3</t>
+  </si>
+  <si>
+    <t>LINAN2</t>
+  </si>
+  <si>
+    <t>LOPE</t>
+  </si>
+  <si>
+    <t>LOPU3</t>
+  </si>
+  <si>
+    <t>MUFI2</t>
+  </si>
+  <si>
+    <t>PHHE2</t>
+  </si>
+  <si>
+    <t>RAOC</t>
+  </si>
+  <si>
+    <t>RAOR3</t>
+  </si>
+  <si>
+    <t>ROWO</t>
+  </si>
+  <si>
+    <t>ROGY</t>
+  </si>
+  <si>
+    <t>RUCA3</t>
+  </si>
+  <si>
+    <t>SCMI2</t>
+  </si>
+  <si>
+    <t>SISYR</t>
+  </si>
+  <si>
+    <t>SOCA6</t>
+  </si>
+  <si>
+    <t>TRIFO</t>
+  </si>
+  <si>
+    <t>TRER2</t>
+  </si>
+  <si>
+    <t>TRRE3</t>
+  </si>
+  <si>
+    <t>SEIN2</t>
+  </si>
+  <si>
+    <t>AGCA5</t>
+  </si>
+  <si>
+    <t>ASCA</t>
+  </si>
+  <si>
+    <t>ASCA2</t>
+  </si>
+  <si>
+    <t>CAAU</t>
+  </si>
+  <si>
+    <t>COGR16</t>
+  </si>
+  <si>
+    <t>CRCA</t>
+  </si>
+  <si>
+    <t>EPAN</t>
+  </si>
+  <si>
+    <t>EPDE2</t>
+  </si>
+  <si>
+    <t>ERAL</t>
+  </si>
+  <si>
+    <t>HYFO7</t>
+  </si>
+  <si>
+    <t>POBI5</t>
+  </si>
+  <si>
+    <t>RUOC</t>
+  </si>
+  <si>
+    <t>CAAU3</t>
+  </si>
+  <si>
+    <t>CRCA3</t>
+  </si>
+  <si>
+    <t>EPAN2</t>
+  </si>
+  <si>
+    <t>EPDE</t>
+  </si>
+  <si>
+    <t>ERAL3</t>
+  </si>
+  <si>
+    <t>RUOC2</t>
+  </si>
+  <si>
+    <t>POLYG4</t>
+  </si>
+  <si>
+    <t>COGR4</t>
+  </si>
+  <si>
+    <t>MAGL</t>
+  </si>
+  <si>
+    <t>MAGL2</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -64,13 +392,26 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="1">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -362,36 +703,461 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:B55"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A50" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B55" sqref="B55"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A1" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="B2" t="s">
+      <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
+      <c r="B2" s="1" t="s">
+        <v>45</v>
+      </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="B3" t="s">
-        <v>2</v>
+      <c r="A3" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="B4" t="s">
-        <v>2</v>
+      <c r="A4" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A5" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A6" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A7" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A8" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A9" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A10" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A11" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A12" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A13" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A14" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A15" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A16" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A17" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A18" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A19" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A20" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A21" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A22" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A23" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A24" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A25" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A26" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A27" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A28" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A29" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A30" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A31" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A32" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A33" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A34" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A35" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A36" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A37" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A38" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A39" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A40" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A41" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A42" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A43" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B43" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A44" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B44" s="1" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A45" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B45" s="1" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A46" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B46" s="1" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A47" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="B47" s="1" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A48" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B48" s="1" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A49" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B49" s="1" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A50" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B50" s="1" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A51" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B51" s="1" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A52" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B52" s="1" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A53" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B53" s="1" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A54" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B54" s="1" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A55" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="B55" s="1" t="s">
+        <v>107</v>
       </c>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="B29">
+    <cfRule type="expression" dxfId="0" priority="1">
+      <formula>$H$29</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>

</xml_diff>